<commit_message>
sql fundamental & release redcarpet
</commit_message>
<xml_diff>
--- a/file/account47.xlsx
+++ b/file/account47.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STU\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lasto\Documents\GitHub\lastone9182.github.io\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="15" windowWidth="14415" windowHeight="12675"/>
+    <workbookView xWindow="-15" yWindow="15" windowWidth="10830" windowHeight="5910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="요약" sheetId="18" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="161">
   <si>
     <t>휴대폰번호</t>
   </si>
@@ -708,6 +708,66 @@
   </si>
   <si>
     <t>기본자본</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박진규</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>비</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보충</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤승업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤성민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유진혁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지각</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지각</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1393,8 +1453,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="data" displayName="data" ref="A1:H9" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:H9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="data" displayName="data" ref="A1:H14" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="이름" dataDxfId="20"/>
     <tableColumn id="2" name="조" dataDxfId="19">
@@ -1418,8 +1478,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="data5" displayName="data5" ref="A1:C3" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="data5" displayName="data5" ref="A1:C4" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
     <tableColumn id="1" name="내용" dataDxfId="12"/>
     <tableColumn id="3" name="날짜" dataDxfId="11"/>
@@ -1734,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1751,7 +1811,7 @@
       </c>
       <c r="B2" s="50">
         <f>SUM(개인별내역!F:F)</f>
-        <v>41000</v>
+        <v>71000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1760,7 +1820,7 @@
       </c>
       <c r="B3" s="50">
         <f>SUM(개인별내역!H:H)</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1769,7 +1829,7 @@
       </c>
       <c r="B4" s="52">
         <f>SUM(지출내용!C:C)</f>
-        <v>-15300</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -1778,7 +1838,7 @@
       </c>
       <c r="B5" s="51">
         <f>B2-B3-B4</f>
-        <v>46300</v>
+        <v>27300</v>
       </c>
     </row>
   </sheetData>
@@ -1790,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1852,18 +1912,18 @@
         <v>42397</v>
       </c>
       <c r="E2" s="39" t="str">
-        <f>IF(D2&lt;&gt;0,VLOOKUP(WEEKDAY(D2,2),weekday,2,FALSE),"")</f>
+        <f t="shared" ref="E2:E9" si="0">IF(D2&lt;&gt;0,VLOOKUP(WEEKDAY(D2,2),weekday,2,FALSE),"")</f>
         <v>목</v>
       </c>
       <c r="F2" s="50">
-        <f>IF(C2&lt;&gt;0,IF(E2="월",VLOOKUP(C2,cost,2,FALSE)*2,VLOOKUP(C2,cost,2,FALSE)),"")</f>
+        <f t="shared" ref="F2:F9" si="1">IF(C2&lt;&gt;0,IF(E2="월",VLOOKUP(C2,cost,2,FALSE)*2,VLOOKUP(C2,cost,2,FALSE)),"")</f>
         <v>5000</v>
       </c>
       <c r="G2" s="50">
         <v>5000</v>
       </c>
       <c r="H2" s="50">
-        <f t="shared" ref="H2:H6" si="0">F2-G2</f>
+        <f t="shared" ref="H2:H6" si="2">F2-G2</f>
         <v>0</v>
       </c>
       <c r="J2"/>
@@ -1883,18 +1943,18 @@
         <v>42397</v>
       </c>
       <c r="E3" s="39" t="str">
-        <f>IF(D3&lt;&gt;0,VLOOKUP(WEEKDAY(D3,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>목</v>
       </c>
       <c r="F3" s="50">
-        <f>IF(C3&lt;&gt;0,IF(E3="월",VLOOKUP(C3,cost,2,FALSE)*2,VLOOKUP(C3,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G3" s="50">
         <v>5000</v>
       </c>
       <c r="H3" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J3"/>
@@ -1914,18 +1974,18 @@
         <v>42397</v>
       </c>
       <c r="E4" s="39" t="str">
-        <f>IF(D4&lt;&gt;0,VLOOKUP(WEEKDAY(D4,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>목</v>
       </c>
       <c r="F4" s="50">
-        <f>IF(C4&lt;&gt;0,IF(E4="월",VLOOKUP(C4,cost,2,FALSE)*2,VLOOKUP(C4,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G4" s="50">
         <v>5000</v>
       </c>
       <c r="H4" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J4"/>
@@ -1945,18 +2005,18 @@
         <v>42398</v>
       </c>
       <c r="E5" s="39" t="str">
-        <f>IF(D5&lt;&gt;0,VLOOKUP(WEEKDAY(D5,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>금</v>
       </c>
       <c r="F5" s="50">
-        <f>IF(C5&lt;&gt;0,IF(E5="월",VLOOKUP(C5,cost,2,FALSE)*2,VLOOKUP(C5,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G5" s="50">
         <v>5000</v>
       </c>
       <c r="H5" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J5"/>
@@ -1976,18 +2036,18 @@
         <v>42401</v>
       </c>
       <c r="E6" s="39" t="str">
-        <f>IF(D6&lt;&gt;0,VLOOKUP(WEEKDAY(D6,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>월</v>
       </c>
       <c r="F6" s="50">
-        <f>IF(C6&lt;&gt;0,IF(E6="월",VLOOKUP(C6,cost,2,FALSE)*2,VLOOKUP(C6,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G6" s="50">
         <v>10000</v>
       </c>
       <c r="H6" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J6"/>
@@ -2007,17 +2067,19 @@
         <v>42401</v>
       </c>
       <c r="E7" s="39" t="str">
-        <f>IF(D7&lt;&gt;0,VLOOKUP(WEEKDAY(D7,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>월</v>
       </c>
       <c r="F7" s="50">
-        <f>IF(C7&lt;&gt;0,IF(E7="월",VLOOKUP(C7,cost,2,FALSE)*2,VLOOKUP(C7,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="50">
+        <v>10000</v>
+      </c>
       <c r="H7" s="50">
-        <f>F7-G7</f>
-        <v>10000</v>
+        <f t="shared" ref="H7:H13" si="3">F7-G7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2035,18 +2097,18 @@
         <v>42397</v>
       </c>
       <c r="E8" s="39" t="str">
-        <f>IF(D8&lt;&gt;0,VLOOKUP(WEEKDAY(D8,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>목</v>
       </c>
       <c r="F8" s="50">
-        <f>IF(C8&lt;&gt;0,IF(E8="월",VLOOKUP(C8,cost,2,FALSE)*2,VLOOKUP(C8,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="G8" s="50">
         <v>500</v>
       </c>
       <c r="H8" s="50">
-        <f>F8-G8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2065,41 +2127,171 @@
         <v>42397</v>
       </c>
       <c r="E9" s="39" t="str">
-        <f>IF(D9&lt;&gt;0,VLOOKUP(WEEKDAY(D9,2),weekday,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>목</v>
       </c>
       <c r="F9" s="50">
-        <f>IF(C9&lt;&gt;0,IF(E9="월",VLOOKUP(C9,cost,2,FALSE)*2,VLOOKUP(C9,cost,2,FALSE)),"")</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="G9" s="50">
         <v>500</v>
       </c>
       <c r="H9" s="50">
-        <f>F9-G9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="39" t="str">
+        <f>VLOOKUP(A10,주소록!$A$2:$D$28,4,FALSE)</f>
+        <v>4조</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="39">
+        <v>42404</v>
+      </c>
+      <c r="E10" s="39" t="str">
+        <f>IF(D10&lt;&gt;0,VLOOKUP(WEEKDAY(D10,2),weekday,2,FALSE),"")</f>
+        <v>목</v>
+      </c>
+      <c r="F10" s="50">
+        <f>IF(C10&lt;&gt;0,IF(E10="월",VLOOKUP(C10,cost,2,FALSE)*2,VLOOKUP(C10,cost,2,FALSE)),"")</f>
+        <v>5000</v>
+      </c>
+      <c r="G10" s="50">
+        <v>5000</v>
+      </c>
+      <c r="H10" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="39" t="str">
+        <f>VLOOKUP(A11,주소록!$A$2:$D$28,4,FALSE)</f>
+        <v>3조</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="39">
+        <v>42415</v>
+      </c>
+      <c r="E11" s="39" t="str">
+        <f>IF(D11&lt;&gt;0,VLOOKUP(WEEKDAY(D11,2),weekday,2,FALSE),"")</f>
+        <v>월</v>
+      </c>
+      <c r="F11" s="50">
+        <f>IF(C11&lt;&gt;0,IF(E11="월",VLOOKUP(C11,cost,2,FALSE)*2,VLOOKUP(C11,cost,2,FALSE)),"")</f>
+        <v>10000</v>
+      </c>
+      <c r="G11" s="50">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="39" t="str">
+        <f>VLOOKUP(A12,주소록!$A$2:$D$28,4,FALSE)</f>
+        <v>5조</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="39">
+        <v>42415</v>
+      </c>
+      <c r="E12" s="39" t="str">
+        <f>IF(D12&lt;&gt;0,VLOOKUP(WEEKDAY(D12,2),weekday,2,FALSE),"")</f>
+        <v>월</v>
+      </c>
+      <c r="F12" s="50">
+        <f>IF(C12&lt;&gt;0,IF(E12="월",VLOOKUP(C12,cost,2,FALSE)*2,VLOOKUP(C12,cost,2,FALSE)),"")</f>
+        <v>10000</v>
+      </c>
+      <c r="G12" s="50">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="39" t="str">
+        <f>VLOOKUP(A13,주소록!$A$2:$D$28,4,FALSE)</f>
+        <v>4조</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="39">
+        <v>42416</v>
+      </c>
+      <c r="E13" s="39" t="str">
+        <f>IF(D13&lt;&gt;0,VLOOKUP(WEEKDAY(D13,2),weekday,2,FALSE),"")</f>
+        <v>화</v>
+      </c>
+      <c r="F13" s="50">
+        <f>IF(C13&lt;&gt;0,IF(E13="월",VLOOKUP(C13,cost,2,FALSE)*2,VLOOKUP(C13,cost,2,FALSE)),"")</f>
+        <v>5000</v>
+      </c>
+      <c r="G13" s="50">
+        <v>5000</v>
+      </c>
+      <c r="H13" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C12 C13">
       <formula1>type</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2140,6 +2332,17 @@
       </c>
       <c r="C3" s="50">
         <v>-28000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="39">
+        <v>42412</v>
+      </c>
+      <c r="C4" s="50">
+        <v>59000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>